<commit_message>
Update surface analysis results with values for BM model
</commit_message>
<xml_diff>
--- a/OIEC_SURFACE-analysis-results_1.xlsx
+++ b/OIEC_SURFACE-analysis-results_1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
   <si>
     <t>Parameter</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>θ</t>
+  </si>
+  <si>
+    <t>2PC BM analysis</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -341,6 +344,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1271,7 +1277,7 @@
         <v>8.6472299999999997E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -1288,11 +1294,119 @@
     <row r="35" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>-173.88333800000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16.8" x14ac:dyDescent="0.75">
+      <c r="A46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>1.3899999999999999E-4</v>
+      </c>
+      <c r="C47">
+        <v>3.2000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>